<commit_message>
browser closed, added dates
</commit_message>
<xml_diff>
--- a/TestArbitr.xlsx
+++ b/TestArbitr.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416D0F03-E1CB-43A1-A67A-09056F1E53DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E37CDCD-B85A-4401-90FA-7053F859F6AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13788" windowHeight="8688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Параметры" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -365,18 +367,18 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -390,30 +392,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>5048028638</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="2">
+        <v>36914</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43458</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>7838412492</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="2">
+        <v>32885</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43366</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>